<commit_message>
this time the code is working and is saying and eveyrhting is fine backend fournt end both , need to make it fast and make the changes in the excel saving formation and many more thats the problem for tommorow so lets sleep now it is 23,54 in the morning 19-08-2025  good night
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -7,16 +7,18 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="www.crystalhues.com_" sheetId="1" r:id="rId1"/>
-    <sheet name="example.com" sheetId="2" r:id="rId2"/>
-    <sheet name="Summary" sheetId="3" r:id="rId3"/>
+    <sheet name="studio-9302.onrender.com" sheetId="1" r:id="rId1"/>
+    <sheet name="studio-9302.onrender.com_produc" sheetId="2" r:id="rId2"/>
+    <sheet name="studio-9302.onrender.com_" sheetId="3" r:id="rId3"/>
+    <sheet name="Common Data" sheetId="4" r:id="rId4"/>
+    <sheet name="Summary" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="98">
   <si>
     <t>URL</t>
   </si>
@@ -33,164 +35,283 @@
     <t>Word Count</t>
   </si>
   <si>
-    <t>https://www.crystalhues.com/</t>
-  </si>
-  <si>
-    <t>Localization Services India | Interpretation Company | Crystal Hues</t>
-  </si>
-  <si>
-    <t>h1</t>
-  </si>
-  <si>
-    <t>h2</t>
-  </si>
-  <si>
-    <t>h3</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>div_col_justify-content-between</t>
-  </si>
-  <si>
-    <t>div_row_highlihts_box_justify-content-between</t>
-  </si>
-  <si>
-    <t>div_row_justify-content-between</t>
-  </si>
-  <si>
-    <t>div_col_justify-content-center</t>
-  </si>
-  <si>
-    <t>div_row_serivese_text_justify-content-between</t>
-  </si>
-  <si>
-    <t>div_col_justify-content-center_testim_slider</t>
-  </si>
-  <si>
-    <t>meta_description</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>Best Localization Company In India - Crystal Hues Ltd</t>
-  </si>
-  <si>
-    <t>Expertise In All Localisation Services</t>
-  </si>
-  <si>
-    <t>Big Or Small, We Help Businesses Of Every Shape &amp; Size</t>
-  </si>
-  <si>
-    <t>We Take Pride In Our Work, And The Testimonial Strengthen Our Resolve</t>
-  </si>
-  <si>
-    <t>Interested In Our Services? Get An Instant Estimate.</t>
-  </si>
-  <si>
-    <t>ISO Certified</t>
-  </si>
-  <si>
-    <t>Highest Quality</t>
-  </si>
-  <si>
-    <t>Fastest Deliveries</t>
-  </si>
-  <si>
-    <t>TRANSLATION</t>
-  </si>
-  <si>
-    <t>TRANSCRIPTION</t>
-  </si>
-  <si>
-    <t>INTERPRETATION</t>
-  </si>
-  <si>
-    <t>"Thanks you very much! Appreciate working and sharing files over the weekend!"</t>
-  </si>
-  <si>
-    <t>"Thanks for all your team support and valuable interactions whenever needed in 2021. We are very happy to have CHL as a translation vendor partner for our major translation work."</t>
-  </si>
-  <si>
-    <t>"It was a very positive experience working with the team of CHL. The task that was assigned to them was done with the greatest perfection. All the specifications that were mentioned in the initial draft for the translation task were followed to the point. We are very satisfied with their performance."</t>
-  </si>
-  <si>
-    <t>WANT TO GET AN ESTIMATE FOR YOUR REQUIREMENT? CLICK ON THE LINK AND GET AN INSTANT ESTIMATE FOR YOUR REQUIREMENTS</t>
-  </si>
-  <si>
-    <t>The best practices welded into workflow system and processes, which are ISO 17100, ISO 18587 certified by ATC Certifications, UK (the first in India), along with ISO 9001 and ISO 27001 certifications.</t>
-  </si>
-  <si>
-    <t>Committed to creating value for our customers by delivering high-quality marketing localization services through well-defined and constantly upgraded processes and methodologies, which ensures consistently meeting and exceeding customer expectations by continually improving the effectiveness of the Quality Management System and other industry-specific international standards.</t>
-  </si>
-  <si>
-    <t>We understand the importance of time, especially when it comes to your projects. We take pride in boasting our accomplishments of delivering projects within timelines with the help of our vast network of more than 500 linguists who are tied up with us across the globe to help us deliver massive projects within extremely tight deadlines without compromising on the quality.</t>
-  </si>
-  <si>
-    <t>Crystal Hues is a public limited 35 years-old ISO certified contentlocalization agencythat has helped some of the biggest brands around the world in overcoming language and cultural barriers. With 6 offices in South-East Asia &amp; 33 back captive offices around the world, and a vast network of 1000+ linguists around the globe, Crystal Hues delivers the highest quality of localized content in the fastest turnaround time.</t>
-  </si>
-  <si>
-    <t>Our prices, though comparable to freelancers, include quality control processes, know-how, and dedicated professionals with the domain expertise to ensure high-quality deliveries. A partial list of clients includes Accenture, Amway, Bates, BBC, Canon, DY&amp;R, GE, Gillette, Hughes, Infosys, KPMG, Lafarge, Star TV, US Government, Virgin Atlantic, WHO, World Bank, etc.</t>
-  </si>
-  <si>
-    <t>The company believes in keeping up to the technology-enabled times and boasts automations and technology support through Artificial Intelligence and Machine Learning softwares like SDL Trados and proprietary ERP systems-driven processes to prove efficiency in operations.</t>
-  </si>
-  <si>
-    <t>Crystal Hues Limitedis committed to creating value for our customers by delivering high-quality marketing communication services through well-defined and constantly upgraded processes and methodologies, which ensures consistently meeting and exceeding customer expectations by continually improving the effectiveness of the Quality Management System and other industry-specific international standards.</t>
-  </si>
-  <si>
-    <t>The linguistic needs of a business are many. You may need ourtranslation servicesto translate a training module for your off-shore employees, or you may need ourinterpretation servicesfor your global conferences. Whatever is your need, Crystal Hues gives a customized solution.With our services, you can reach people across the world.</t>
-  </si>
-  <si>
-    <t>For over 35 years, we've been like a lighthouse guiding many great companies in their communication journey.It's with their trust in our abilities and world-class service delivery we're at the top of our industry.Here are some of our valuable clients who traveled with us along our journey to the top.</t>
-  </si>
-  <si>
-    <t>Are you looking for a collaboration with us? Want to know the specific details of how we work and what we bring to the table?Just input your requirements and get an instant quote. CHL always adheres to transparency and fair business practices.And the results you are seeking, you'll get the best!</t>
-  </si>
-  <si>
-    <t>WANT TO GET AN ESTIMATE FOR YOUR REQUIREMENT? CLICK ON THE LINK AND GET AN INSTANT ESTIMATE FOR YOUR REQUIREMENTSGET AN INSTANT QUOTE</t>
-  </si>
-  <si>
-    <t>ISO CertifiedThe best practices welded into workflow system and processes, which are ISO 17100, ISO 18587 certified by ATC Certifications, UK (the first in India), along with ISO 9001 and ISO 27001 certifications.Highest QualityCommitted to creating value for our customers by delivering high-quality marketing localization services through well-defined and constantly upgraded processes and methodologies, which ensures consistently meeting and exceeding customer expectations by continually improving the effectiveness of the Quality Management System and other industry-specific international standards.Fastest DeliveriesWe understand the importance of time, especially when it comes to your projects. We take pride in boasting our accomplishments of delivering projects within timelines with the help of our vast network of more than 500 linguists who are tied up with us across the globe to help us deliver massive projects within extremely tight deadlines without compromising on the quality.</t>
-  </si>
-  <si>
-    <t>Best Localization Company In India - Crystal Hues LtdCrystal Hues is a public limited 35 years-old ISO certified contentlocalization agencythat has helped some of the biggest brands around the world in overcoming language and cultural barriers. With 6 offices in South-East Asia &amp; 33 back captive offices around the world, and a vast network of 1000+ linguists around the globe, Crystal Hues delivers the highest quality of localized content in the fastest turnaround time.Our prices, though comparable to freelancers, include quality control processes, know-how, and dedicated professionals with the domain expertise to ensure high-quality deliveries. A partial list of clients includes Accenture, Amway, Bates, BBC, Canon, DY&amp;R, GE, Gillette, Hughes, Infosys, KPMG, Lafarge, Star TV, US Government, Virgin Atlantic, WHO, World Bank, etc.The company believes in keeping up to the technology-enabled times and boasts automations and technology support through Artificial Intelligence and Machine Learning softwares like SDL Trados and proprietary ERP systems-driven processes to prove efficiency in operations.Crystal Hues Limitedis committed to creating value for our customers by delivering high-quality marketing communication services through well-defined and constantly upgraded processes and methodologies, which ensures consistently meeting and exceeding customer expectations by continually improving the effectiveness of the Quality Management System and other industry-specific international standards.</t>
-  </si>
-  <si>
-    <t>Expertise In All Localisation ServicesThe linguistic needs of a business are many. You may need ourtranslation servicesto translate a training module for your off-shore employees, or you may need ourinterpretation servicesfor your global conferences. Whatever is your need, Crystal Hues gives a customized solution.With our services, you can reach people across the world.</t>
-  </si>
-  <si>
-    <t>TRANSLATIONTRANSCRIPTIONINTERPRETATIONVOICE-OVERSUBTITLING</t>
-  </si>
-  <si>
-    <t>Big Or Small, We Help Businesses Of Every Shape &amp; SizeFor over 35 years, we've been like a lighthouse guiding many great companies in their communication journey.It's with their trust in our abilities and world-class service delivery we're at the top of our industry.Here are some of our valuable clients who traveled with us along our journey to the top.View All Clients</t>
-  </si>
-  <si>
-    <t>"Thanks you very much! Appreciate working and sharing files over the weekend!"- Colleen,Bain &amp; Company"Thanks for all your team support and valuable interactions whenever needed in 2021. We are very happy to have CHL as a translation vendor partner for our major translation work."- Ramdas Giri"It was a very positive experience working with the team of CHL. The task that was assigned to them was done with the greatest perfection. All the specifications that were mentioned in the initial draft for the translation task were followed to the point. We are very satisfied with their performance."- Laith Kubba</t>
-  </si>
-  <si>
-    <t>Interested In Our Services? Get An Instant Estimate.Are you looking for a collaboration with us? Want to know the specific details of how we work and what we bring to the table?Just input your requirements and get an instant quote. CHL always adheres to transparency and fair business practices.And the results you are seeking, you'll get the best!CONTACT US</t>
-  </si>
-  <si>
-    <t>Crystal Hues is an ISO-certified localization company providing accurate translation, transcription, voiceover, and interpretation services in India.</t>
+    <t>https://studio-9302.onrender.com</t>
+  </si>
+  <si>
+    <t>Spec Showdown</t>
+  </si>
+  <si>
+    <t>h2_text-3xl_font-headline_font-bold</t>
+  </si>
+  <si>
+    <t>h2_text-3xl_font-headline_font-bold_mb-6</t>
+  </si>
+  <si>
+    <t>p_text-sm_text-muted-foreground</t>
+  </si>
+  <si>
+    <t>div_min-h-screen_bg-background_text-foreground</t>
+  </si>
+  <si>
+    <t>div_rounded-lg_border_bg-card_text-card-foreground_shadow-sm_flex_flex-col_h-full_transition-all_duration-300_cursor-pointer_hover:shadow-xl_hover:-translate-y-1</t>
+  </si>
+  <si>
+    <t>div_font-semibold_tracking-tight_font-headline_text-lg_h-14</t>
+  </si>
+  <si>
+    <t>div_rounded-lg_border_bg-card_text-card-foreground_shadow-lg</t>
+  </si>
+  <si>
+    <t>div_text-sm_text-muted-foreground</t>
+  </si>
+  <si>
+    <t>div_flex_justify-between_items-baseline_font-bold_text-lg</t>
+  </si>
+  <si>
+    <t>div_rounded-lg_border_text-card-foreground_shadow-sm_bg-secondary/30_dark:bg-card_mt-4</t>
+  </si>
+  <si>
+    <t>div_font-semibold_tracking-tight_text-base_flex_items-center_gap-2</t>
+  </si>
+  <si>
+    <t>div_p-4_pt-0_text-sm</t>
+  </si>
+  <si>
+    <t>div_rounded-lg_border_text-card-foreground_shadow-sm_bg-secondary/50_dark:bg-card_mt-4</t>
+  </si>
+  <si>
+    <t>div_text-2xl_font-semibold_leading-none_tracking-tight_flex_items-center_gap-2</t>
+  </si>
+  <si>
+    <t>div_rounded-lg_border_bg-card_text-card-foreground_shadow-sm_mt-8</t>
+  </si>
+  <si>
+    <t>div_text-2xl_font-semibold_leading-none_tracking-tight_font-headline_flex_items-center_gap-4</t>
+  </si>
+  <si>
+    <t>span_font-semibold_text-foreground</t>
+  </si>
+  <si>
+    <t>span_font-mono_text-primary_whitespace-nowrap</t>
+  </si>
+  <si>
+    <t>td_p-4_align-middle_[&amp;:has([role=checkbox])]:pr-0</t>
+  </si>
+  <si>
+    <t>th_h-12_px-4_text-left_align-middle_text-muted-foreground_[&amp;:has([role=checkbox])]:pr-0_font-bold_min-w-[200px]</t>
+  </si>
+  <si>
+    <t>Featured Laptop</t>
+  </si>
+  <si>
+    <t>Choose Your Peripherals</t>
+  </si>
+  <si>
+    <t>Click the button to get your personalized financing recommendation based on your total cost.</t>
+  </si>
+  <si>
+    <t>Featured LaptopChange LaptopLegion Pro 7 Intel₹2,65,843CPU:Intel Core UltraGPU:NVIDIA RTX 4080RAM:32GB DDR5Storage:2TB SSDDisplay:16" WQXGAShop NowChoose Your PeripheralsThinkVision M14t Gen 2₹29,990Type:Portable MonitorSize:14 inch TouchResolution:2240x1400Refresh Rate:60HzShop NowRazer Basilisk V3 Pro₹12,000Type:Wireless MouseSensor:OpticalDPI:30,000Buttons:11 ProgrammableShop NowHive65 Mechanical Keyboard₹3,000Type:Mechanical KeyboardSwitch:Kreo Purple SwitchesLayout:65% CompactBacklight:RGBShop NowArctik Laptop Cooler₹3,000Type:Cooling PadFan Speed:Up to 2400 RPMNoise Level:25 dBALighting:RGBShop NowYour SetupReview your selections and total cost.Legion Pro 7 Intel₹2,65,843.00Total Cost₹2,65,843.00EMI for Total Setup12 Months:₹23,994.54/mo18 Months:₹16,584.56/mo24 Months:₹12,889.84/moAI Financing AssistantGet AI-powered advice on how to finance your purchase.Click the button to get your personalized financing recommendation based on your total cost.Get Financing AdviceAI Laptop ComparisonSide-by-side comparison of your selected laptop and AI-powered suggestions from the web.FeatureASUS ROG Strix Scar 16 (2024)MSI Raider GE78HX 14VJLenovo Legion 9i (16")Price₹2,70,990₹2,64,990₹2,59,990CPUIntel Core i9-14900HXIntel Core i9-14900HXIntel Core i9-14900HXGPUNVIDIA RTX 4080NVIDIA RTX 4080NVIDIA GeForce RTX 4080RAM32GB DDR532GB DDR532GB DDR5Storage1TB SSD2TB SSD1TB SSDDisplay16" QHD+ 240Hz17" QHD+ 240Hz16" Mini-LED 165HzShop NowShop NowShop Now</t>
+  </si>
+  <si>
+    <t>ThinkVision M14t Gen 2₹29,990Type:Portable MonitorSize:14 inch TouchResolution:2240x1400Refresh Rate:60HzShop Now</t>
+  </si>
+  <si>
+    <t>ThinkVision M14t Gen 2</t>
+  </si>
+  <si>
+    <t>Razer Basilisk V3 Pro₹12,000Type:Wireless MouseSensor:OpticalDPI:30,000Buttons:11 ProgrammableShop Now</t>
+  </si>
+  <si>
+    <t>Razer Basilisk V3 Pro</t>
+  </si>
+  <si>
+    <t>Hive65 Mechanical Keyboard₹3,000Type:Mechanical KeyboardSwitch:Kreo Purple SwitchesLayout:65% CompactBacklight:RGBShop Now</t>
+  </si>
+  <si>
+    <t>Hive65 Mechanical Keyboard</t>
+  </si>
+  <si>
+    <t>Arctik Laptop Cooler₹3,000Type:Cooling PadFan Speed:Up to 2400 RPMNoise Level:25 dBALighting:RGBShop Now</t>
+  </si>
+  <si>
+    <t>Arctik Laptop Cooler</t>
+  </si>
+  <si>
+    <t>Your SetupReview your selections and total cost.Legion Pro 7 Intel₹2,65,843.00Total Cost₹2,65,843.00EMI for Total Setup12 Months:₹23,994.54/mo18 Months:₹16,584.56/mo24 Months:₹12,889.84/moAI Financing AssistantGet AI-powered advice on how to finance your purchase.Click the button to get your personalized financing recommendation based on your total cost.Get Financing Advice</t>
+  </si>
+  <si>
+    <t>Review your selections and total cost.</t>
+  </si>
+  <si>
+    <t>Total Cost₹2,65,843.00</t>
+  </si>
+  <si>
+    <t>EMI for Total Setup12 Months:₹23,994.54/mo18 Months:₹16,584.56/mo24 Months:₹12,889.84/mo</t>
+  </si>
+  <si>
+    <t>EMI for Total Setup</t>
+  </si>
+  <si>
+    <t>12 Months:₹23,994.54/mo18 Months:₹16,584.56/mo24 Months:₹12,889.84/mo</t>
+  </si>
+  <si>
+    <t>AI Financing AssistantGet AI-powered advice on how to finance your purchase.Click the button to get your personalized financing recommendation based on your total cost.Get Financing Advice</t>
+  </si>
+  <si>
+    <t>AI Financing Assistant</t>
+  </si>
+  <si>
+    <t>Get AI-powered advice on how to finance your purchase.</t>
+  </si>
+  <si>
+    <t>AI Laptop ComparisonSide-by-side comparison of your selected laptop and AI-powered suggestions from the web.FeatureASUS ROG Strix Scar 16 (2024)MSI Raider GE78HX 14VJLenovo Legion 9i (16")Price₹2,70,990₹2,64,990₹2,59,990CPUIntel Core i9-14900HXIntel Core i9-14900HXIntel Core i9-14900HXGPUNVIDIA RTX 4080NVIDIA RTX 4080NVIDIA GeForce RTX 4080RAM32GB DDR532GB DDR532GB DDR5Storage1TB SSD2TB SSD1TB SSDDisplay16" QHD+ 240Hz17" QHD+ 240Hz16" Mini-LED 165HzShop NowShop NowShop Now</t>
+  </si>
+  <si>
+    <t>AI Laptop Comparison</t>
+  </si>
+  <si>
+    <t>Side-by-side comparison of your selected laptop and AI-powered suggestions from the web.</t>
+  </si>
+  <si>
+    <t>Resolution:</t>
+  </si>
+  <si>
+    <t>Refresh Rate:</t>
+  </si>
+  <si>
+    <t>Noise Level:</t>
+  </si>
+  <si>
+    <t>₹2,65,843.00</t>
+  </si>
+  <si>
+    <t>Intel Core i9-14900HX</t>
+  </si>
+  <si>
+    <t>NVIDIA RTX 4080</t>
+  </si>
+  <si>
+    <t>NVIDIA GeForce RTX 4080</t>
+  </si>
+  <si>
+    <t>16" QHD+ 240Hz</t>
+  </si>
+  <si>
+    <t>17" QHD+ 240Hz</t>
+  </si>
+  <si>
+    <t>16" Mini-LED 165Hz</t>
+  </si>
+  <si>
+    <t>ASUS ROG Strix Scar 16 (2024)</t>
+  </si>
+  <si>
+    <t>MSI Raider GE78HX 14VJ</t>
+  </si>
+  <si>
+    <t>Lenovo Legion 9i (16")</t>
   </si>
   <si>
     <t>Total Words</t>
   </si>
   <si>
-    <t>https://example.com</t>
-  </si>
-  <si>
-    <t>Example Domain</t>
-  </si>
-  <si>
-    <t>This domain is for use in illustrative examples in documents. You may use this
-    domain in literature without prior coordination or asking for permission.</t>
-  </si>
-  <si>
-    <t>More information...</t>
+    <t>https://studio-9302.onrender.com/products</t>
+  </si>
+  <si>
+    <t>h1_text-3xl_md:text-4xl_font-bold_font-headline_text-primary_ml-4</t>
+  </si>
+  <si>
+    <t>p_text-2xl_font-bold_text-primary_mt-2</t>
+  </si>
+  <si>
+    <t>div_rounded-lg_border_bg-card_text-card-foreground_shadow-sm_flex_flex-col_h-full_transition-all_duration-300</t>
+  </si>
+  <si>
+    <t>Choose a Laptop</t>
+  </si>
+  <si>
+    <t>₹1,32,789.98</t>
+  </si>
+  <si>
+    <t>Choose a LaptopLegion Pro 7 Intel₹2,65,843CPU:Intel Core UltraGPU:NVIDIA RTX 4080RAM:32GB DDR5Storage:2TB SSDDisplay:16" WQXGAShop NowLenovo Legion 5 15IRX9₹1,22,990CPU:Intel Core i7 13th GenGPU:NVIDIA RTX 4060RAM:24GB DDR5Storage:512GB SSDDisplay:15.6" FHD 144HzShop NowMSI Sword 16 HX₹1,39,990CPU:Intel Core i9 14th GenGPU:NVIDIA RTX 4060RAM:16GB DDR5Storage:1TB SSDDisplay:16" FHD+ 144HzShop NowHP Omen 16 xd0020AX₹1,04,490CPU:AMD Ryzen 7GPU:NVIDIA RTX 4060RAM:16GB DDR5Storage:1TB SSDDisplay:16.1" FHD 165HzShop NowLenovo LOQ Gen 9₹94,990CPU:AMD Ryzen 7GPU:NVIDIA RTX 4050RAM:16GB DDR5Storage:512GB SSDDisplay:15.6" FHDShop NowAlienware 16 Aurora₹1,32,789.98CPU:Intel Core i7GPU:NVIDIA RTX 4060RAM:16GB DDR5Storage:1TB SSDDisplay:16" QHD+ 240HzShop Now</t>
+  </si>
+  <si>
+    <t>Lenovo Legion 5 15IRX9₹1,22,990CPU:Intel Core i7 13th GenGPU:NVIDIA RTX 4060RAM:24GB DDR5Storage:512GB SSDDisplay:15.6" FHD 144HzShop Now</t>
+  </si>
+  <si>
+    <t>Lenovo Legion 5 15IRX9</t>
+  </si>
+  <si>
+    <t>MSI Sword 16 HX₹1,39,990CPU:Intel Core i9 14th GenGPU:NVIDIA RTX 4060RAM:16GB DDR5Storage:1TB SSDDisplay:16" FHD+ 144HzShop Now</t>
+  </si>
+  <si>
+    <t>MSI Sword 16 HX</t>
+  </si>
+  <si>
+    <t>HP Omen 16 xd0020AX₹1,04,490CPU:AMD Ryzen 7GPU:NVIDIA RTX 4060RAM:16GB DDR5Storage:1TB SSDDisplay:16.1" FHD 165HzShop Now</t>
+  </si>
+  <si>
+    <t>HP Omen 16 xd0020AX</t>
+  </si>
+  <si>
+    <t>Lenovo LOQ Gen 9₹94,990CPU:AMD Ryzen 7GPU:NVIDIA RTX 4050RAM:16GB DDR5Storage:512GB SSDDisplay:15.6" FHDShop Now</t>
+  </si>
+  <si>
+    <t>Lenovo LOQ Gen 9</t>
+  </si>
+  <si>
+    <t>Alienware 16 Aurora₹1,32,789.98CPU:Intel Core i7GPU:NVIDIA RTX 4060RAM:16GB DDR5Storage:1TB SSDDisplay:16" QHD+ 240HzShop Now</t>
+  </si>
+  <si>
+    <t>Alienware 16 Aurora</t>
+  </si>
+  <si>
+    <t>https://studio-9302.onrender.com/</t>
+  </si>
+  <si>
+    <t>Featured LaptopChange LaptopLegion Pro 7 Intel₹2,65,843CPU:Intel Core UltraGPU:NVIDIA RTX 4080RAM:32GB DDR5Storage:2TB SSDDisplay:16" WQXGAShop NowChoose Your PeripheralsThinkVision M14t Gen 2₹29,990Type:Portable MonitorSize:14 inch TouchResolution:2240x1400Refresh Rate:60HzShop NowRazer Basilisk V3 Pro₹12,000Type:Wireless MouseSensor:OpticalDPI:30,000Buttons:11 ProgrammableShop NowHive65 Mechanical Keyboard₹3,000Type:Mechanical KeyboardSwitch:Kreo Purple SwitchesLayout:65% CompactBacklight:RGBShop NowArctik Laptop Cooler₹3,000Type:Cooling PadFan Speed:Up to 2400 RPMNoise Level:25 dBALighting:RGBShop NowYour SetupReview your selections and total cost.Legion Pro 7 Intel₹2,65,843.00Total Cost₹2,65,843.00EMI for Total Setup12 Months:₹23,994.54/mo18 Months:₹16,584.56/mo24 Months:₹12,889.84/moAI Financing AssistantGet AI-powered advice on how to finance your purchase.Click the button to get your personalized financing recommendation based on your total cost.Get Financing AdviceAI Laptop ComparisonSide-by-side comparison of your selected laptop and AI-powered suggestions from the web.FeatureASUS ROG Strix SCAR 16 (2024)MSI Raider GE78HX 14VJLenovo Legion 9i (16") Gen 9Price₹2,74,990₹2,69,990₹2,59,999CPUIntel Core i9-14900HXIntel Core i9-14900HXIntel Core i9-14900HXGPUNVIDIA GeForce RTX 4080NVIDIA GeForce RTX 4080NVIDIA GeForce RTX 4080RAM32GB DDR532GB DDR532GB DDR5Storage1TB PCIe Gen4 SSD2TB NVMe PCIe Gen4 SSD1TB NVMe PCIe Gen4 SSDDisplay16-inch QHD+ 240Hz17-inch QHD+ 240Hz16-inch Mini-LED 165HzShop NowShop NowShop Now</t>
+  </si>
+  <si>
+    <t>AI Laptop ComparisonSide-by-side comparison of your selected laptop and AI-powered suggestions from the web.FeatureASUS ROG Strix SCAR 16 (2024)MSI Raider GE78HX 14VJLenovo Legion 9i (16") Gen 9Price₹2,74,990₹2,69,990₹2,59,999CPUIntel Core i9-14900HXIntel Core i9-14900HXIntel Core i9-14900HXGPUNVIDIA GeForce RTX 4080NVIDIA GeForce RTX 4080NVIDIA GeForce RTX 4080RAM32GB DDR532GB DDR532GB DDR5Storage1TB PCIe Gen4 SSD2TB NVMe PCIe Gen4 SSD1TB NVMe PCIe Gen4 SSDDisplay16-inch QHD+ 240Hz17-inch QHD+ 240Hz16-inch Mini-LED 165HzShop NowShop NowShop Now</t>
+  </si>
+  <si>
+    <t>1TB PCIe Gen4 SSD</t>
+  </si>
+  <si>
+    <t>2TB NVMe PCIe Gen4 SSD</t>
+  </si>
+  <si>
+    <t>1TB NVMe PCIe Gen4 SSD</t>
+  </si>
+  <si>
+    <t>16-inch QHD+ 240Hz</t>
+  </si>
+  <si>
+    <t>17-inch QHD+ 240Hz</t>
+  </si>
+  <si>
+    <t>16-inch Mini-LED 165Hz</t>
+  </si>
+  <si>
+    <t>ASUS ROG Strix SCAR 16 (2024)</t>
+  </si>
+  <si>
+    <t>Lenovo Legion 9i (16") Gen 9</t>
+  </si>
+  <si>
+    <t>URLs</t>
+  </si>
+  <si>
+    <t>Legion Pro 7 Intel₹2,65,843CPU:Intel Core UltraGPU:NVIDIA RTX 4080RAM:32GB DDR5Storage:2TB SSDDisplay:16" WQXGAShop Now</t>
+  </si>
+  <si>
+    <t>Legion Pro 7 Intel</t>
+  </si>
+  <si>
+    <t>Compare laptops and peripherals to build your perfect setup.</t>
+  </si>
+  <si>
+    <t>['https://studio-9302.onrender.com', 'https://studio-9302.onrender.com/products', 'https://studio-9302.onrender.com/']</t>
   </si>
 </sst>
 </file>
@@ -561,7 +682,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -595,10 +716,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E2">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -612,10 +733,10 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -626,13 +747,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E4">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -643,13 +764,13 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E5">
-        <v>12</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -660,13 +781,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -677,13 +798,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -694,13 +815,13 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -711,13 +832,13 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -728,13 +849,13 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -745,13 +866,13 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -762,13 +883,13 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -779,13 +900,13 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E13">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -796,13 +917,13 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E14">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -813,13 +934,13 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E15">
-        <v>51</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -830,13 +951,13 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E16">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -847,13 +968,13 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E17">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -864,13 +985,13 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E18">
-        <v>44</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -881,13 +1002,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E19">
-        <v>61</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -898,13 +1019,13 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E20">
-        <v>66</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -915,13 +1036,13 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E21">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -932,13 +1053,13 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E22">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -949,13 +1070,13 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E23">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -966,13 +1087,13 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E24">
-        <v>49</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -983,13 +1104,13 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E25">
-        <v>50</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1000,13 +1121,13 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E26">
-        <v>51</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1017,13 +1138,13 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E27">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1034,13 +1155,13 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E28">
-        <v>138</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1051,13 +1172,13 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E29">
-        <v>204</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1068,13 +1189,13 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E30">
-        <v>53</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1085,13 +1206,13 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1102,13 +1223,13 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E32">
-        <v>62</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1119,13 +1240,13 @@
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E33">
-        <v>98</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1136,13 +1257,13 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E34">
-        <v>59</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1153,13 +1274,13 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E35">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1170,21 +1291,55 @@
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E36">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" t="s">
-        <v>53</v>
+      <c r="A37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
       </c>
       <c r="E37">
-        <v>1317</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39">
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -1224,6 +1379,8 @@
     <hyperlink ref="A34" r:id="rId33"/>
     <hyperlink ref="A35" r:id="rId34"/>
     <hyperlink ref="A36" r:id="rId35"/>
+    <hyperlink ref="A37" r:id="rId36"/>
+    <hyperlink ref="A38" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1231,7 +1388,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1256,16 +1413,290 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A14" r:id="rId13"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1273,44 +1704,810 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="E3">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
         <v>54</v>
       </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41">
+        <v>455</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A14" r:id="rId13"/>
+    <hyperlink ref="A15" r:id="rId14"/>
+    <hyperlink ref="A16" r:id="rId15"/>
+    <hyperlink ref="A17" r:id="rId16"/>
+    <hyperlink ref="A18" r:id="rId17"/>
+    <hyperlink ref="A19" r:id="rId18"/>
+    <hyperlink ref="A20" r:id="rId19"/>
+    <hyperlink ref="A21" r:id="rId20"/>
+    <hyperlink ref="A22" r:id="rId21"/>
+    <hyperlink ref="A23" r:id="rId22"/>
+    <hyperlink ref="A24" r:id="rId23"/>
+    <hyperlink ref="A25" r:id="rId24"/>
+    <hyperlink ref="A26" r:id="rId25"/>
+    <hyperlink ref="A27" r:id="rId26"/>
+    <hyperlink ref="A28" r:id="rId27"/>
+    <hyperlink ref="A29" r:id="rId28"/>
+    <hyperlink ref="A30" r:id="rId29"/>
+    <hyperlink ref="A31" r:id="rId30"/>
+    <hyperlink ref="A32" r:id="rId31"/>
+    <hyperlink ref="A33" r:id="rId32"/>
+    <hyperlink ref="A34" r:id="rId33"/>
+    <hyperlink ref="A35" r:id="rId34"/>
+    <hyperlink ref="A36" r:id="rId35"/>
+    <hyperlink ref="A37" r:id="rId36"/>
+    <hyperlink ref="A38" r:id="rId37"/>
+    <hyperlink ref="A39" r:id="rId38"/>
+    <hyperlink ref="A40" r:id="rId39"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
       <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4">
+        <v>97</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5">
-        <v>28</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4">
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -1321,45 +2518,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>1317</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>